<commit_message>
Updated: * FuseSheetsTask * FuseSheetsView * XlsxSheetReader
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -21,21 +21,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
-  <si>
-    <t xml:space="preserve">Имя</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Фамилия</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Отчество</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Возраст</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Адрес</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="107">
+  <si>
+    <t xml:space="preserve">Firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patronymic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
   </si>
   <si>
     <t xml:space="preserve">Name1</t>
@@ -48,6 +51,9 @@
   </si>
   <si>
     <t xml:space="preserve">address1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coolname123@email.com</t>
   </si>
   <si>
     <t xml:space="preserve">Name2</t>
@@ -433,13 +439,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.17"/>
@@ -461,433 +467,538 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>9</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>13</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>14</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>15</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>17</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>38</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>18</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>19</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>46</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>20</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>21</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>54</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>22</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>58</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>23</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>62</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>24</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>25</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>70</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>26</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>74</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>27</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>78</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>28</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>82</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>29</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>86</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>30</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>31</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>94</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>32</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>98</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>33</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>102</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>34</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="coolname123@email.com"/>
+    <hyperlink ref="F3" r:id="rId2" display="coolname123@email.com"/>
+    <hyperlink ref="F4" r:id="rId3" display="coolname123@email.com"/>
+    <hyperlink ref="F5" r:id="rId4" display="coolname123@email.com"/>
+    <hyperlink ref="F6" r:id="rId5" display="coolname123@email.com"/>
+    <hyperlink ref="F7" r:id="rId6" display="coolname123@email.com"/>
+    <hyperlink ref="F8" r:id="rId7" display="coolname123@email.com"/>
+    <hyperlink ref="F9" r:id="rId8" display="coolname123@email.com"/>
+    <hyperlink ref="F10" r:id="rId9" display="coolname123@email.com"/>
+    <hyperlink ref="F11" r:id="rId10" display="coolname123@email.com"/>
+    <hyperlink ref="F12" r:id="rId11" display="coolname123@email.com"/>
+    <hyperlink ref="F13" r:id="rId12" display="coolname123@email.com"/>
+    <hyperlink ref="F14" r:id="rId13" display="coolname123@email.com"/>
+    <hyperlink ref="F15" r:id="rId14" display="coolname123@email.com"/>
+    <hyperlink ref="F16" r:id="rId15" display="coolname123@email.com"/>
+    <hyperlink ref="F17" r:id="rId16" display="coolname123@email.com"/>
+    <hyperlink ref="F18" r:id="rId17" display="coolname123@email.com"/>
+    <hyperlink ref="F19" r:id="rId18" display="coolname123@email.com"/>
+    <hyperlink ref="F20" r:id="rId19" display="coolname123@email.com"/>
+    <hyperlink ref="F21" r:id="rId20" display="coolname123@email.com"/>
+    <hyperlink ref="F22" r:id="rId21" display="coolname123@email.com"/>
+    <hyperlink ref="F23" r:id="rId22" display="coolname123@email.com"/>
+    <hyperlink ref="F24" r:id="rId23" display="coolname123@email.com"/>
+    <hyperlink ref="F25" r:id="rId24" display="coolname123@email.com"/>
+    <hyperlink ref="F26" r:id="rId25" display="coolname123@email.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -909,7 +1020,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Fixes: * SheetsLogger * XlsxSheetReader - added Field's validation method support
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="108">
   <si>
     <t xml:space="preserve">Firstname</t>
   </si>
@@ -53,19 +53,22 @@
     <t xml:space="preserve">address1</t>
   </si>
   <si>
+    <t xml:space="preserve">peepeepoopoo123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surname2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lastname2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address2</t>
+  </si>
+  <si>
     <t xml:space="preserve">coolname123@email.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Surname2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lastname2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">address2</t>
   </si>
   <si>
     <t xml:space="preserve">Name3</t>
@@ -442,7 +445,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -471,7 +474,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
@@ -508,204 +511,204 @@
         <v>14</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>13</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>14</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>15</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>16</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>17</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>18</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>19</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>20</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>21</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>10</v>
@@ -713,291 +716,289 @@
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>22</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>23</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>24</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>25</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>26</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>27</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>28</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>29</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>30</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>31</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>32</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>33</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>34</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="coolname123@email.com"/>
-    <hyperlink ref="F3" r:id="rId2" display="coolname123@email.com"/>
-    <hyperlink ref="F4" r:id="rId3" display="coolname123@email.com"/>
-    <hyperlink ref="F5" r:id="rId4" display="coolname123@email.com"/>
-    <hyperlink ref="F6" r:id="rId5" display="coolname123@email.com"/>
-    <hyperlink ref="F7" r:id="rId6" display="coolname123@email.com"/>
-    <hyperlink ref="F8" r:id="rId7" display="coolname123@email.com"/>
-    <hyperlink ref="F9" r:id="rId8" display="coolname123@email.com"/>
-    <hyperlink ref="F10" r:id="rId9" display="coolname123@email.com"/>
-    <hyperlink ref="F11" r:id="rId10" display="coolname123@email.com"/>
-    <hyperlink ref="F12" r:id="rId11" display="coolname123@email.com"/>
-    <hyperlink ref="F13" r:id="rId12" display="coolname123@email.com"/>
-    <hyperlink ref="F14" r:id="rId13" display="coolname123@email.com"/>
-    <hyperlink ref="F15" r:id="rId14" display="coolname123@email.com"/>
-    <hyperlink ref="F16" r:id="rId15" display="coolname123@email.com"/>
-    <hyperlink ref="F17" r:id="rId16" display="coolname123@email.com"/>
-    <hyperlink ref="F18" r:id="rId17" display="coolname123@email.com"/>
-    <hyperlink ref="F19" r:id="rId18" display="coolname123@email.com"/>
-    <hyperlink ref="F20" r:id="rId19" display="coolname123@email.com"/>
-    <hyperlink ref="F21" r:id="rId20" display="coolname123@email.com"/>
-    <hyperlink ref="F22" r:id="rId21" display="coolname123@email.com"/>
-    <hyperlink ref="F23" r:id="rId22" display="coolname123@email.com"/>
-    <hyperlink ref="F24" r:id="rId23" display="coolname123@email.com"/>
-    <hyperlink ref="F25" r:id="rId24" display="coolname123@email.com"/>
-    <hyperlink ref="F26" r:id="rId25" display="coolname123@email.com"/>
+    <hyperlink ref="F3" r:id="rId1" display="coolname123@email.com"/>
+    <hyperlink ref="F4" r:id="rId2" display="coolname123@email.com"/>
+    <hyperlink ref="F5" r:id="rId3" display="coolname123@email.com"/>
+    <hyperlink ref="F6" r:id="rId4" display="coolname123@email.com"/>
+    <hyperlink ref="F7" r:id="rId5" display="coolname123@email.com"/>
+    <hyperlink ref="F8" r:id="rId6" display="coolname123@email.com"/>
+    <hyperlink ref="F9" r:id="rId7" display="coolname123@email.com"/>
+    <hyperlink ref="F10" r:id="rId8" display="coolname123@email.com"/>
+    <hyperlink ref="F11" r:id="rId9" display="coolname123@email.com"/>
+    <hyperlink ref="F12" r:id="rId10" display="coolname123@email.com"/>
+    <hyperlink ref="F14" r:id="rId11" display="coolname123@email.com"/>
+    <hyperlink ref="F15" r:id="rId12" display="coolname123@email.com"/>
+    <hyperlink ref="F16" r:id="rId13" display="coolname123@email.com"/>
+    <hyperlink ref="F17" r:id="rId14" display="coolname123@email.com"/>
+    <hyperlink ref="F18" r:id="rId15" display="coolname123@email.com"/>
+    <hyperlink ref="F19" r:id="rId16" display="coolname123@email.com"/>
+    <hyperlink ref="F20" r:id="rId17" display="coolname123@email.com"/>
+    <hyperlink ref="F21" r:id="rId18" display="coolname123@email.com"/>
+    <hyperlink ref="F22" r:id="rId19" display="coolname123@email.com"/>
+    <hyperlink ref="F23" r:id="rId20" display="coolname123@email.com"/>
+    <hyperlink ref="F24" r:id="rId21" display="coolname123@email.com"/>
+    <hyperlink ref="F25" r:id="rId22" display="coolname123@email.com"/>
+    <hyperlink ref="F26" r:id="rId23" display="coolname123@email.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
* New reader based on pylightxl
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -9,7 +9,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -453,7 +452,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1096,27 +1095,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>